<commit_message>
Att Organizador e Pastas
</commit_message>
<xml_diff>
--- a/Tabelas Consulta/Banco de Dados/banco de dados - CEIMIC.xlsx
+++ b/Tabelas Consulta/Banco de Dados/banco de dados - CEIMIC.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Vitor\Programacao\teste_CEIMIC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://servmar365-my.sharepoint.com/personal/henrique_canhadas_servmarambiental_com/Documents/Documentos/Codigos/GitHub Tecnologia/ProjetoCanhadas/Tabelas Consulta/Banco de Dados/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{000B2C6E-E2EE-4C1D-B15E-A419BFEE3E00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
@@ -3861,9 +3861,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office 2013 - 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -3901,7 +3901,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -4007,7 +4007,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -4149,7 +4149,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -4159,8 +4159,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D704"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A455" workbookViewId="0">
+      <selection activeCell="B478" sqref="B478"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>

</xml_diff>